<commit_message>
Algorithms for recommendation systems in C#.
</commit_message>
<xml_diff>
--- a/docs/epinions.results.xlsx
+++ b/docs/epinions.results.xlsx
@@ -428,6 +428,289 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{20452C02-BDD4-44D1-8E61-0EBCE30665BB}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1DF0AD22-64CC-4857-B05D-BE0C5B4CD0D8}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7296ADE5-B616-4ABE-95B7-8AA5D03BC01F}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{698B21CC-CDD4-4329-A564-F084CE63D496}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{912F2677-89EE-42B6-B242-70FB29F6D731}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BCD8AA8B-4FBE-456F-B36C-51672BE58DA4}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E8576574-D6C4-484D-9084-13B5BE0A97BE}" type="CELLRANGE">
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$K$97:$K$103</c:f>
@@ -489,6 +772,37 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$J$97:$J$103</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>30</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -498,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1526512784"/>
-        <c:axId val="1526514416"/>
+        <c:axId val="-191262480"/>
+        <c:axId val="-191267376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1526512784"/>
+        <c:axId val="-191262480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +873,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1526514416"/>
+        <c:crossAx val="-191267376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -597,7 +911,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1526514416"/>
+        <c:axId val="-191267376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +968,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1526512784"/>
+        <c:crossAx val="-191262480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1297,13 +1611,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>704851</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
       <xdr:row>132</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
@@ -1616,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="O122" sqref="O122"/>
     </sheetView>
   </sheetViews>

</xml_diff>